<commit_message>
the roll command now semi works
</commit_message>
<xml_diff>
--- a/Book.xlsx
+++ b/Book.xlsx
@@ -14,7 +14,10 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="28">
+  <si>
+    <t>Id</t>
+  </si>
   <si>
     <t>Name</t>
   </si>
@@ -152,11 +155,11 @@
   </cellStyleXfs>
   <cellXfs count="7">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
     </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -164,11 +167,11 @@
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -185,15 +188,16 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:F10" displayName="Table1" name="Table1" id="1" totalsRowShown="0">
-  <autoFilter ref="A1:F10"/>
-  <tableColumns count="6">
-    <tableColumn name="Name" id="1"/>
-    <tableColumn name="Anime" id="2"/>
-    <tableColumn name="Power" id="3"/>
-    <tableColumn name="Type" id="4"/>
-    <tableColumn name="Rarity" id="5"/>
-    <tableColumn name="Image" id="6"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:G6" displayName="Table1" name="Table1" id="1" totalsRowShown="0">
+  <autoFilter ref="A1:G6"/>
+  <tableColumns count="7">
+    <tableColumn name="Id" id="1"/>
+    <tableColumn name="Name" id="2"/>
+    <tableColumn name="Anime" id="3"/>
+    <tableColumn name="Power" id="4"/>
+    <tableColumn name="Type" id="5"/>
+    <tableColumn name="Rarity" id="6"/>
+    <tableColumn name="Image" id="7"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showColumnStripes="0" showRowStripes="1" showLastColumn="0" showFirstColumn="0"/>
 </table>
@@ -487,25 +491,26 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:F10"/>
+  <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" style="5" width="15.290714285714287" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="5" width="24.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="6" width="24.576428571428572" customWidth="1" bestFit="1"/>
     <col min="3" max="3" style="6" width="11.43357142857143" customWidth="1" bestFit="1"/>
     <col min="4" max="4" style="5" width="11.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="5" width="11.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="5" width="11.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="6" width="11.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="6" width="11.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="6" width="13.576428571428572" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
@@ -514,144 +519,130 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="2" t="s">
         <v>5</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>6</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
-      <c r="A2" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B2" s="1" t="s">
+      <c r="A2" s="3">
+        <v>0</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="3">
+      <c r="C2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="3">
         <v>120</v>
       </c>
-      <c r="D2" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E2" s="1" t="s">
+      <c r="E2" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="F2" s="2" t="s">
         <v>10</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>11</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
-      <c r="A3" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B3" s="1" t="s">
+      <c r="A3" s="3">
+        <v>1</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="3">
+      <c r="C3" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" s="3">
         <v>240</v>
       </c>
-      <c r="D3" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="F3" s="1" t="s">
+      <c r="E3" s="2" t="s">
         <v>14</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>15</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5">
-      <c r="A4" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="B4" s="1" t="s">
+      <c r="A4" s="3">
+        <v>2</v>
+      </c>
+      <c r="B4" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="C4" s="3">
+      <c r="C4" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D4" s="3">
         <v>230</v>
       </c>
-      <c r="D4" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="F4" s="1" t="s">
+      <c r="E4" s="2" t="s">
         <v>18</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>19</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
-      <c r="A5" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B5" s="1" t="s">
+      <c r="A5" s="3">
+        <v>3</v>
+      </c>
+      <c r="B5" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C5" s="3">
+      <c r="C5" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D5" s="3">
         <v>160</v>
       </c>
-      <c r="D5" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="F5" s="1" t="s">
+      <c r="E5" s="2" t="s">
         <v>22</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>23</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
-      <c r="A6" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B6" s="1" t="s">
+      <c r="A6" s="3">
+        <v>4</v>
+      </c>
+      <c r="B6" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="C6" s="3">
+      <c r="C6" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D6" s="3">
         <v>250</v>
       </c>
-      <c r="D6" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="F6" s="1" t="s">
+      <c r="E6" s="2" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18.75">
-      <c r="A7" s="1"/>
-      <c r="B7" s="1"/>
-      <c r="C7" s="2"/>
-      <c r="D7" s="1"/>
-      <c r="E7" s="1"/>
-      <c r="F7" s="1"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18.75">
-      <c r="A8" s="1"/>
-      <c r="B8" s="1"/>
-      <c r="C8" s="2"/>
-      <c r="D8" s="1"/>
-      <c r="E8" s="1"/>
-      <c r="F8" s="1"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18.75">
-      <c r="A9" s="1"/>
-      <c r="B9" s="1"/>
-      <c r="C9" s="2"/>
-      <c r="D9" s="1"/>
-      <c r="E9" s="1"/>
-      <c r="F9" s="1"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="18.75">
-      <c r="A10" s="1"/>
-      <c r="B10" s="1"/>
-      <c r="C10" s="2"/>
-      <c r="D10" s="1"/>
-      <c r="E10" s="1"/>
-      <c r="F10" s="1"/>
+      <c r="F6" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>27</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>